<commit_message>
chore: More WIP on search page
</commit_message>
<xml_diff>
--- a/seed/software.xlsx
+++ b/seed/software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerburguillos/AIMS-Project/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21216496-F863-7C45-84F8-156E8334EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84271C13-98B1-1841-900D-450C6734EFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{153D47C6-62AB-FF4E-B429-DB56BB55003C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{153D47C6-62AB-FF4E-B429-DB56BB55003C}"/>
   </bookViews>
   <sheets>
     <sheet name="software" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <t>Software</t>
   </si>
@@ -371,6 +371,15 @@
   </si>
   <si>
     <t>Replaced legacy Office 2016 license</t>
+  </si>
+  <si>
+    <t>Microsoft Internet Explorer Premium Edition</t>
+  </si>
+  <si>
+    <t>Y2K-2000</t>
+  </si>
+  <si>
+    <t>Internet Explorer: Still downloading; finally gave up.</t>
   </si>
 </sst>
 </file>
@@ -406,9 +415,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,21 +735,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8314B780-760F-424F-993A-138500FEF07B}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2030,11 +2043,50 @@
       <c r="K34" t="s">
         <v>111</v>
       </c>
-      <c r="L34" t="b">
+      <c r="L34" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1994</v>
+      </c>
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>0.01</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>114</v>
+      </c>
+      <c r="L35" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>